<commit_message>
PROS-6604 - MARSRU - Development
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_SAND/Data/2019/KPIs for DB - MARS KPIs.xlsx
+++ b/Projects/MARSRU_SAND/Data/2019/KPIs for DB - MARS KPIs.xlsx
@@ -145,8 +145,7 @@
     <t xml:space="preserve">Категория тов. для животных примыкает к ЦЕНТРАЛЬНОЙ АЛЛЕЕ и визуально доступна покупателям по ходу их движения без необходимости оборачиваться</t>
   </si>
   <si>
-    <t xml:space="preserve">Категория товаров для животных примыкает к ПРОМО АЛЛЕЕ, находится дальше 5-ти метров от входа и визуально доступна покупателям по ходу их движения без необходимости оборачиваться 
-</t>
+    <t xml:space="preserve">Категория товаров для животных примыкает к ПРОМО АЛЛЕЕ, находится дальше 5-ти метров от входа и визуально доступна покупателям по ходу их движения без необходимости оборачиваться </t>
   </si>
   <si>
     <t xml:space="preserve">Ассортимент для Котят/Щенков, а также Senior сгруппирован (влажный и сухой) и располагается внутри соответствующих бренд блоков </t>
@@ -300,18 +299,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="227.908163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.7142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="225.301020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -328,7 +328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -342,7 +342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
@@ -356,7 +356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
@@ -370,7 +370,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
@@ -384,7 +384,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>4</v>
       </c>
@@ -398,7 +398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>4</v>
       </c>
@@ -412,7 +412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>4</v>
       </c>
@@ -426,7 +426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>4</v>
       </c>
@@ -440,7 +440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>4</v>
       </c>
@@ -454,7 +454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>4</v>
       </c>
@@ -468,7 +468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>4</v>
       </c>
@@ -482,7 +482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>4</v>
       </c>
@@ -496,7 +496,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>4</v>
       </c>
@@ -510,7 +510,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>4</v>
       </c>
@@ -524,7 +524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>4</v>
       </c>
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>4</v>
       </c>
@@ -552,7 +552,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>4</v>
       </c>
@@ -566,7 +566,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>4</v>
       </c>
@@ -580,7 +580,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>4</v>
       </c>
@@ -594,7 +594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>4</v>
       </c>
@@ -608,7 +608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>4</v>
       </c>
@@ -622,7 +622,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>4</v>
       </c>
@@ -636,7 +636,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>4</v>
       </c>
@@ -650,7 +650,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>4</v>
       </c>
@@ -664,7 +664,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>4</v>
       </c>
@@ -678,7 +678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>4</v>
       </c>
@@ -692,7 +692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>4</v>
       </c>
@@ -706,7 +706,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>4</v>
       </c>
@@ -720,7 +720,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>4</v>
       </c>
@@ -734,7 +734,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>4</v>
       </c>
@@ -748,7 +748,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>4</v>
       </c>
@@ -762,7 +762,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>4</v>
       </c>
@@ -776,7 +776,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>4</v>
       </c>
@@ -790,7 +790,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>4</v>
       </c>
@@ -804,7 +804,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>4</v>
       </c>
@@ -818,7 +818,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>4</v>
       </c>
@@ -832,7 +832,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>4</v>
       </c>
@@ -874,7 +874,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>4</v>
       </c>
@@ -888,7 +888,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>4</v>
       </c>
@@ -902,7 +902,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>4</v>
       </c>
@@ -916,7 +916,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>4</v>
       </c>
@@ -930,7 +930,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>4</v>
       </c>
@@ -944,7 +944,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>4</v>
       </c>
@@ -958,7 +958,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>4</v>
       </c>
@@ -972,7 +972,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>4</v>
       </c>
@@ -986,7 +986,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>4</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>4</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>4</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>4</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>4</v>
       </c>
@@ -1056,6 +1056,22 @@
         <v>56</v>
       </c>
     </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>